<commit_message>
refactoring and fix bugs
</commit_message>
<xml_diff>
--- a/fitnesStudioModul/src/main/resources/templates/excelExample.xlsx
+++ b/fitnesStudioModul/src/main/resources/templates/excelExample.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Download\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\JetBrains\Projects\FitnessStudio\fitnesStudioModul\src\main\resources\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E00FDF0E-6101-42DE-8068-50B8EE3F5B63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBACB662-86B5-49AB-B09B-22ED35C39A02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -82,12 +82,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -405,7 +404,7 @@
   <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -431,19 +430,19 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
       <c r="I1" s="1" t="s">

</xml_diff>